<commit_message>
Pooh Points: normal 20260129
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-01-29.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-01-29.xlsx
@@ -429,7 +429,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="26" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
@@ -530,7 +530,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Booz</t>
+          <t>Boozers Losers</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -591,7 +591,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Booz</t>
+          <t>Boozers Losers</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -652,7 +652,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Booz</t>
+          <t>Boozers Losers</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Booz</t>
+          <t>Boozers Losers</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -774,7 +774,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Booz</t>
+          <t>Boozers Losers</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -835,7 +835,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CDL</t>
+          <t>The Backslashers</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CDL</t>
+          <t>The Backslashers</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -957,7 +957,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CDL</t>
+          <t>The Backslashers</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CDL</t>
+          <t>The Backslashers</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CDL</t>
+          <t>The Backslashers</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>CDL</t>
+          <t>The Backslashers</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CDL</t>
+          <t>The Backslashers</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Clay</t>
+          <t>Hilton Heads</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Clay</t>
+          <t>Hilton Heads</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Clay</t>
+          <t>Hilton Heads</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Hal</t>
+          <t>Three Dawg Nite</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Hal</t>
+          <t>Three Dawg Nite</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1567,7 +1567,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Hal</t>
+          <t>Three Dawg Nite</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Hal</t>
+          <t>Three Dawg Nite</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1689,7 +1689,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Hal</t>
+          <t>Three Dawg Nite</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1750,7 +1750,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Bend Rimmers</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Bend Rimmers</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1872,7 +1872,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Bend Rimmers</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Bend Rimmers</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1994,7 +1994,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Bend Rimmers</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -2055,7 +2055,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Bend Rimmers</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Ron</t>
+          <t>G-Flop</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2177,7 +2177,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Ron</t>
+          <t>G-Flop</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2238,7 +2238,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Ron</t>
+          <t>G-Flop</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Ron</t>
+          <t>G-Flop</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2360,7 +2360,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Ron</t>
+          <t>G-Flop</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Ron</t>
+          <t>G-Flop</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2482,7 +2482,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Tar</t>
+          <t>The Oddities</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2543,7 +2543,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Tar</t>
+          <t>The Oddities</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2604,7 +2604,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Tar</t>
+          <t>The Oddities</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Tar</t>
+          <t>The Oddities</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Tar</t>
+          <t>The Oddities</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -5421,7 +5421,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="7" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
     <col width="23" customWidth="1" min="3" max="3"/>
   </cols>
@@ -5446,7 +5446,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Ron</t>
+          <t>G-Flop</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -5459,7 +5459,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CDL</t>
+          <t>The Backslashers</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -5472,7 +5472,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Booz</t>
+          <t>Boozers Losers</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -5485,7 +5485,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Clay</t>
+          <t>Hilton Heads</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -5498,7 +5498,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Hal</t>
+          <t>Three Dawg Nite</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -5511,7 +5511,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Bend Rimmers</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -5524,7 +5524,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tar</t>
+          <t>The Oddities</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>